<commit_message>
raw variables added, observed variable description update, python code update
</commit_message>
<xml_diff>
--- a/data/data_20121010.xlsx
+++ b/data/data_20121010.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
-    <t>tau_w_obs</t>
+    <t>nom_w_pc_obs</t>
   </si>
   <si>
     <t>1983Q1</t>
@@ -699,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-0.02100161234673004</v>
+        <v>-0.001963394164474025</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -707,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.02374793170196554</v>
+        <v>-0.002327504873449959</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -715,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-0.06143986003162061</v>
+        <v>-0.008373402913548197</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -723,7 +723,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-0.06357239831402905</v>
+        <v>-0.0002334146387425184</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -731,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-0.05907251970153782</v>
+        <v>-0.004974087501678437</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -739,7 +739,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-0.06350772143113037</v>
+        <v>-0.002873876727537014</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -747,7 +747,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-0.05682762801336017</v>
+        <v>0.001872250636571593</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -755,7 +755,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-0.05095005440377998</v>
+        <v>-0.00228381552655392</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -763,7 +763,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-0.001339777334146808</v>
+        <v>-0.002278336726335276</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -771,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-0.06153142702615289</v>
+        <v>-0.0004924139046595666</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -779,7 +779,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-0.02825651183869105</v>
+        <v>0.006035274326563464</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -787,7 +787,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-0.02579876934652714</v>
+        <v>0.007769347920333403</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -795,7 +795,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-0.0268004195764775</v>
+        <v>0.002415724089875573</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -803,7 +803,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-0.02730809129768352</v>
+        <v>0.00118931654183134</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -811,7 +811,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-0.02220597513886635</v>
+        <v>0.001565370138131392</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -819,7 +819,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>-0.01008153233828835</v>
+        <v>0.001790707291433644</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -827,7 +827,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-0.0252480677443907</v>
+        <v>-0.00694435872936372</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -835,7 +835,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.02665900374328234</v>
+        <v>-0.002425624942349477</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -843,7 +843,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>-0.0132013840517089</v>
+        <v>-0.001008517241987528</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -851,7 +851,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>-0.008299359107081905</v>
+        <v>0.001184001079845579</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -859,7 +859,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>-0.005119404015464291</v>
+        <v>0.006224470727149073</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -867,7 +867,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-0.02009145999175255</v>
+        <v>-0.0008061487366662068</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -875,7 +875,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>-0.02227231181220635</v>
+        <v>-0.003361268411086568</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -883,7 +883,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-0.02335564757386455</v>
+        <v>-0.004484875849591119</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -891,7 +891,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.006545596189490244</v>
+        <v>-0.01132433911920276</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -899,7 +899,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.0168215675061465</v>
+        <v>-0.01001255424457459</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -907,7 +907,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0.01505056922119974</v>
+        <v>-0.001729372575774657</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -915,7 +915,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.01749506282345847</v>
+        <v>0.004175660861490085</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -923,7 +923,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>0.01491014782221911</v>
+        <v>-0.001575335022303712</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -931,7 +931,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>0.01081322913499583</v>
+        <v>0.007002297589531081</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -939,7 +939,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0.01433259174679979</v>
+        <v>0.003444667621483974</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -947,7 +947,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0.009517749051319191</v>
+        <v>-0.002518721722083173</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -955,7 +955,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>0.0001639963233235342</v>
+        <v>-0.004773396740810676</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -963,7 +963,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>-0.0002561450102585017</v>
+        <v>0.009413578462240307</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -971,7 +971,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>-0.0003396951934835357</v>
+        <v>0.0004995165982373123</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -979,7 +979,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>-0.0004243960673029346</v>
+        <v>0.001965463999947098</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -987,7 +987,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>-0.01663966083148005</v>
+        <v>0.01060139104450275</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -995,7 +995,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-0.0116482575645418</v>
+        <v>-0.0008800727788100815</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1003,7 +1003,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>-0.009703618342804754</v>
+        <v>0.007358359036720559</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1011,7 +1011,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-0.004586834356468339</v>
+        <v>-0.005788029093942874</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1019,7 +1019,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>-0.02312863233554818</v>
+        <v>-0.007631792155466721</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1027,7 +1027,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>-0.008093413687368267</v>
+        <v>-0.004671021829008942</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1035,7 +1035,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.0001626769653837457</v>
+        <v>-0.003510703031341253</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1043,7 +1043,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.003060582841962534</v>
+        <v>-0.004611063363654272</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1051,7 +1051,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>-0.003750073148015343</v>
+        <v>0.002955948045206061</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1059,7 +1059,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>0.007462761013456332</v>
+        <v>-0.009215908231850908</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1067,7 +1067,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>-0.003306604986426764</v>
+        <v>-0.009272178687502755</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1075,7 +1075,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>-0.005259010644925954</v>
+        <v>-0.003046135161522259</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1083,7 +1083,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>0.002449277140551542</v>
+        <v>-0.0003963008488961223</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1091,7 +1091,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>0.01307108251662648</v>
+        <v>-0.001672419281086079</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1099,7 +1099,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.008659965759066024</v>
+        <v>-0.001460118188855108</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1107,7 +1107,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>0.01328134580911788</v>
+        <v>0.000322224279866376</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1115,7 +1115,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>0.02365015837849493</v>
+        <v>0.001359508163468234</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1123,7 +1123,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>0.03651849150042596</v>
+        <v>0.002622025574123513</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1131,7 +1131,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>0.03270434443728742</v>
+        <v>-0.001234995625449209</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1139,7 +1139,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>0.036090081056249</v>
+        <v>-0.004240339388076789</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1147,7 +1147,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>0.04924224340787009</v>
+        <v>-0.004141632451587704</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1155,7 +1155,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>0.05007904795123097</v>
+        <v>0.000610156620693289</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1163,7 +1163,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>0.05290021904967457</v>
+        <v>0.004047255672081682</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1171,7 +1171,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>0.05937515916300695</v>
+        <v>0.01040248382502396</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1179,7 +1179,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>0.06651324905274469</v>
+        <v>0.0145316991866177</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1187,7 +1187,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>0.07020472988318649</v>
+        <v>0.007954394128898014</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1195,7 +1195,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>0.07057131196558619</v>
+        <v>0.008539955473361269</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1203,7 +1203,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>0.07614252633407959</v>
+        <v>-0.002543627116747119</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1211,7 +1211,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>0.07276051646022141</v>
+        <v>0.008302946294300263</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1219,7 +1219,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>0.07466574301693063</v>
+        <v>-0.005348561326916364</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1227,7 +1227,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>0.07921988985438055</v>
+        <v>0.001276359773586241</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1235,7 +1235,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>0.08092142629874322</v>
+        <v>0.01323850717418746</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1243,7 +1243,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>0.09177534561666012</v>
+        <v>0.01415004597231243</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1251,7 +1251,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>0.09293308078043494</v>
+        <v>-0.005583624382106071</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1259,7 +1259,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>0.09308399941936352</v>
+        <v>0.01098340024974537</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1267,7 +1267,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>0.09516211994304014</v>
+        <v>-0.002811435893628575</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1275,7 +1275,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>0.1083009929560959</v>
+        <v>0.01256398819791785</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1283,7 +1283,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>0.1078337773457096</v>
+        <v>-0.007508911314378432</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1291,7 +1291,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>0.02100549258931461</v>
+        <v>-0.003642373631874308</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1299,7 +1299,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>0.07446330895830822</v>
+        <v>0.003188310844850489</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1307,7 +1307,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>-0.002768217016191121</v>
+        <v>0.003596726868077233</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1315,7 +1315,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>-0.0196069685729976</v>
+        <v>0.001951000246955345</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1323,7 +1323,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>-0.0235231212590048</v>
+        <v>-0.002709270498215394</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1331,7 +1331,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>-0.03690665035709317</v>
+        <v>-0.004752789629131809</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1339,7 +1339,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>-0.04922017620070607</v>
+        <v>0.001053642528424417</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1347,7 +1347,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>-0.06244006271310698</v>
+        <v>0.01035110686425354</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1355,7 +1355,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>-0.1077655445690027</v>
+        <v>0.004293346537803751</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1363,7 +1363,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>-0.08279927551526267</v>
+        <v>-0.00115305671897727</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1371,7 +1371,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>-0.08744882487674688</v>
+        <v>-0.01432597766720594</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1379,7 +1379,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>-0.08931521730657477</v>
+        <v>0.002015120475835603</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1387,7 +1387,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>-0.08305824538619611</v>
+        <v>0.004727584164920291</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1395,7 +1395,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>-0.07748454577271491</v>
+        <v>-0.003331277738278505</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1403,7 +1403,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>-0.05207211977576809</v>
+        <v>-0.004862589571685204</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1411,7 +1411,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>-0.04908290019722106</v>
+        <v>-0.003628658572890836</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1419,7 +1419,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>-0.04651381192859616</v>
+        <v>-1.960821037370192e-05</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1427,7 +1427,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>-0.04571086857471451</v>
+        <v>-0.006343162706074861</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1435,7 +1435,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>-0.02396079319755251</v>
+        <v>0.002690668643429795</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1443,7 +1443,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>-0.02499874848377748</v>
+        <v>-0.008187966377292711</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1451,7 +1451,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>-0.02661986138601091</v>
+        <v>-0.008106612773870007</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1459,7 +1459,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>-0.01947277194212482</v>
+        <v>0.01476256641352053</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1467,7 +1467,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>0.01058119221562692</v>
+        <v>-0.006982890863131128</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1475,7 +1475,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>0.0113552070794869</v>
+        <v>-0.006430824044111862</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1483,7 +1483,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>0.01557865491555877</v>
+        <v>-9.805544284256784e-05</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1491,7 +1491,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>0.0157597476526592</v>
+        <v>0.00698338133195929</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1499,7 +1499,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>0.01841037342692631</v>
+        <v>0.00792942162362931</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1507,12 +1507,15 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>-0.04932470498021346</v>
+        <v>-0.01212899702642564</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1" t="s">
         <v>103</v>
+      </c>
+      <c r="B104">
+        <v>-0.002873431204955041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data, and script for KK14, also get_vintage_data.py
</commit_message>
<xml_diff>
--- a/data/data_20121010.xlsx
+++ b/data/data_20121010.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
-    <t>nom_w_pc_obs</t>
+    <t>govdebt_rcpc_obs</t>
   </si>
   <si>
     <t>1983Q1</t>
@@ -699,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-0.001963394164474025</v>
+        <v>0.1261408116688424</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -707,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.002327504873449959</v>
+        <v>0.09353756063987154</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -715,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-0.008373402913548197</v>
+        <v>0.09384950029112429</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -723,7 +723,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-0.0002334146387425184</v>
+        <v>0.07578909220622135</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -731,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-0.004974087501678437</v>
+        <v>0.05384392728215217</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -739,7 +739,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-0.002873876727537014</v>
+        <v>0.05490798724647763</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -747,7 +747,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.001872250636571593</v>
+        <v>0.05213786959980706</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -755,7 +755,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-0.00228381552655392</v>
+        <v>0.0555075466825802</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -763,7 +763,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-0.002278336726335276</v>
+        <v>0.03160103075550027</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -771,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-0.0004924139046595666</v>
+        <v>0.05133398833675931</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -779,7 +779,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.006035274326563464</v>
+        <v>0.03939551562873391</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -787,7 +787,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.007769347920333403</v>
+        <v>0.0364179876403933</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -795,7 +795,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.002415724089875573</v>
+        <v>0.03007042301872578</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -803,7 +803,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.00118931654183134</v>
+        <v>0.03313772103084092</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -811,7 +811,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.001565370138131392</v>
+        <v>0.03302719713448945</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -819,7 +819,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.001790707291433644</v>
+        <v>0.01884574300483135</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -827,7 +827,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-0.00694435872936372</v>
+        <v>0.01684175144963231</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -835,7 +835,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-0.002425624942349477</v>
+        <v>0.007662325536864543</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -843,7 +843,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>-0.001008517241987528</v>
+        <v>0.006539888365702538</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -851,7 +851,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.001184001079845579</v>
+        <v>0.007310038471498047</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -859,7 +859,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.006224470727149073</v>
+        <v>0.003609078723670799</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -867,7 +867,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-0.0008061487366662068</v>
+        <v>0.0001134386481892666</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -875,7 +875,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>-0.003361268411086568</v>
+        <v>-0.005651770378015321</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -883,7 +883,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-0.004484875849591119</v>
+        <v>-0.00119886424152358</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -891,7 +891,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>-0.01132433911920276</v>
+        <v>-0.008269216071823272</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -899,7 +899,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>-0.01001255424457459</v>
+        <v>-0.005154515268939931</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -907,7 +907,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>-0.001729372575774657</v>
+        <v>-0.001238423165013415</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -915,7 +915,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.004175660861490085</v>
+        <v>-0.001409740693218843</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -923,7 +923,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>-0.001575335022303712</v>
+        <v>-0.009179236696036021</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -931,7 +931,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>0.007002297589531081</v>
+        <v>-0.003812588617461678</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -939,7 +939,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0.003444667621483974</v>
+        <v>-0.002726727613686065</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -947,7 +947,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>-0.002518721722083173</v>
+        <v>0.002957800509127438</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -955,7 +955,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>-0.004773396740810676</v>
+        <v>-0.007221190532190704</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -963,7 +963,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>0.009413578462240307</v>
+        <v>0.003434289841226644</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -971,7 +971,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>0.0004995165982373123</v>
+        <v>0.005695085355889383</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -979,7 +979,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>0.001965463999947098</v>
+        <v>0.006015094549419196</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -987,7 +987,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>0.01060139104450275</v>
+        <v>0.009855983884072515</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -995,7 +995,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-0.0008800727788100815</v>
+        <v>0.00922330859072109</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1003,7 +1003,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.007358359036720559</v>
+        <v>0.00995093723119269</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1011,7 +1011,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-0.005788029093942874</v>
+        <v>0.005487405253851073</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1019,7 +1019,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>-0.007631792155466721</v>
+        <v>0.00542943473688564</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1027,7 +1027,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>-0.004671021829008942</v>
+        <v>0.001406276967416041</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1035,7 +1035,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>-0.003510703031341253</v>
+        <v>0.001601895754599035</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1043,7 +1043,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>-0.004611063363654272</v>
+        <v>-0.002750166649822951</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1051,7 +1051,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.002955948045206061</v>
+        <v>-0.005567676091189667</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1059,7 +1059,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>-0.009215908231850908</v>
+        <v>-0.007767653769757167</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1067,7 +1067,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>-0.009272178687502755</v>
+        <v>-0.007188200741892949</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1075,7 +1075,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>-0.003046135161522259</v>
+        <v>-0.007727092537029946</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1083,7 +1083,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>-0.0003963008488961223</v>
+        <v>-0.007204523533620978</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1091,7 +1091,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>-0.001672419281086079</v>
+        <v>-0.008174065050497205</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1099,7 +1099,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>-0.001460118188855108</v>
+        <v>-0.01069349520463034</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1107,7 +1107,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>0.000322224279866376</v>
+        <v>-0.01186743252802933</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1115,7 +1115,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>0.001359508163468234</v>
+        <v>-0.01052187789044488</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1123,7 +1123,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>0.002622025574123513</v>
+        <v>-0.01307135461899232</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1131,7 +1131,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>-0.001234995625449209</v>
+        <v>-0.0159552500397838</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1139,7 +1139,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>-0.004240339388076789</v>
+        <v>-0.01936573506249615</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1147,7 +1147,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>-0.004141632451587704</v>
+        <v>-0.02225760244998063</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1155,7 +1155,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>0.000610156620693289</v>
+        <v>-0.02262002628295998</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1163,7 +1163,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>0.004047255672081682</v>
+        <v>-0.02192668707309529</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1171,7 +1171,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>0.01040248382502396</v>
+        <v>-0.02295937330100038</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1179,7 +1179,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>0.0145316991866177</v>
+        <v>-0.02421747329354793</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1187,7 +1187,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>0.007954394128898014</v>
+        <v>-0.02680865738743186</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1195,7 +1195,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>0.008539955473361269</v>
+        <v>-0.02997475873340192</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1203,7 +1203,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>-0.002543627116747119</v>
+        <v>-0.02916003705531565</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1211,7 +1211,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>0.008302946294300263</v>
+        <v>-0.03372286220034435</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1219,7 +1219,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>-0.005348561326916364</v>
+        <v>-0.03333563999300391</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1227,7 +1227,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>0.001276359773586241</v>
+        <v>-0.03319222732820069</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1235,7 +1235,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>0.01323850717418746</v>
+        <v>-0.03368925618571903</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1243,7 +1243,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>0.01415004597231243</v>
+        <v>-0.05652797037467869</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1251,7 +1251,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>-0.005583624382106071</v>
+        <v>-0.04117613723731437</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1259,7 +1259,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>0.01098340024974537</v>
+        <v>-0.04262647510796067</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1267,7 +1267,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>-0.002811435893628575</v>
+        <v>-0.04158153678582131</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1275,7 +1275,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>0.01256398819791785</v>
+        <v>-0.04181908127961918</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1283,7 +1283,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>-0.007508911314378432</v>
+        <v>-0.038596037427966</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1291,7 +1291,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>-0.003642373631874308</v>
+        <v>-0.01598660192597055</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1299,7 +1299,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>0.003188310844850489</v>
+        <v>-0.02335102372976414</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1307,7 +1307,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>0.003596726868077233</v>
+        <v>-0.007228579935758851</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1315,7 +1315,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>0.001951000246955345</v>
+        <v>-0.004529302573401985</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1323,7 +1323,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>-0.002709270498215394</v>
+        <v>-0.004294746697896513</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1331,7 +1331,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>-0.004752789629131809</v>
+        <v>-0.00277811403998416</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1339,7 +1339,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>0.001053642528424417</v>
+        <v>-0.008614446755511686</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1347,7 +1347,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>0.01035110686425354</v>
+        <v>0.005705856502581284</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1355,7 +1355,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>0.004293346537803751</v>
+        <v>0.007383173408631948</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1363,7 +1363,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>-0.00115305671897727</v>
+        <v>0.000661995384704149</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1371,7 +1371,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>-0.01432597766720594</v>
+        <v>0.001856653328962253</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1379,7 +1379,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>0.002015120475835603</v>
+        <v>-0.003242639865522846</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1387,7 +1387,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>0.004727584164920291</v>
+        <v>-0.00363266611469313</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1395,7 +1395,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>-0.003331277738278505</v>
+        <v>-0.005093233057539372</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1403,7 +1403,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>-0.004862589571685204</v>
+        <v>-0.01088737402535443</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1411,7 +1411,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>-0.003628658572890836</v>
+        <v>-0.008998977569558121</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1419,7 +1419,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>-1.960821037370192e-05</v>
+        <v>-0.009610680291573061</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1427,7 +1427,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>-0.006343162706074861</v>
+        <v>-0.01303141121175187</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1435,7 +1435,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>0.002690668643429795</v>
+        <v>-0.01464895280416232</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1443,7 +1443,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>-0.008187966377292711</v>
+        <v>-0.01540808523565693</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1451,7 +1451,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>-0.008106612773870007</v>
+        <v>-0.01548267581010285</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1459,7 +1459,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>0.01476256641352053</v>
+        <v>-0.01816524297492648</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1467,7 +1467,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>-0.006982890863131128</v>
+        <v>-0.02107375400066789</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1475,7 +1475,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>-0.006430824044111862</v>
+        <v>-0.01318356937406171</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1483,7 +1483,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>-9.805544284256784e-05</v>
+        <v>-0.008231480558097949</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1491,7 +1491,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>0.00698338133195929</v>
+        <v>-0.009630314692508392</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1499,7 +1499,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>0.00792942162362931</v>
+        <v>-0.002522855657092073</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1507,15 +1507,12 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>-0.01212899702642564</v>
+        <v>0.01124975073282699</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B104">
-        <v>-0.002873431204955041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>